<commit_message>
Week 2 Queue Ques Part 2
Week 2 Queue Ques Part 2
</commit_message>
<xml_diff>
--- a/Week 2/Week 2 Questions.xlsx
+++ b/Week 2/Week 2 Questions.xlsx
@@ -69,10 +69,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -96,6 +96,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -104,30 +126,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,22 +144,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -205,6 +197,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -220,21 +219,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -255,49 +255,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,7 +405,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -321,115 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,32 +460,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -538,6 +512,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -546,157 +535,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -710,6 +710,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1034,7 +1037,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1077,12 +1080,12 @@
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="3:3">
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1092,12 +1095,12 @@
       </c>
     </row>
     <row r="9" spans="3:3">
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="3:3">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1107,12 +1110,12 @@
       </c>
     </row>
     <row r="12" spans="3:3">
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="3:3">
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>